<commit_message>
Update for first draft
</commit_message>
<xml_diff>
--- a/data/a_acv.xlsx
+++ b/data/a_acv.xlsx
@@ -14,24 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Algorithm</t>
   </si>
   <si>
-    <t>One Year Alt</t>
-  </si>
-  <si>
-    <t>Two Year Alt</t>
-  </si>
-  <si>
-    <t>Three Year Alt</t>
-  </si>
-  <si>
-    <t>Five Year Alt</t>
-  </si>
-  <si>
-    <t>Ten Year Alt</t>
+    <t>One Year Alt mean</t>
+  </si>
+  <si>
+    <t>One Year Alt std</t>
+  </si>
+  <si>
+    <t>Two Year Alt mean</t>
+  </si>
+  <si>
+    <t>Two Year Alt std</t>
+  </si>
+  <si>
+    <t>Three Year Alt mean</t>
+  </si>
+  <si>
+    <t>Three Year Alt std</t>
+  </si>
+  <si>
+    <t>Five Year Alt mean</t>
+  </si>
+  <si>
+    <t>Five Year Alt std</t>
+  </si>
+  <si>
+    <t>Ten Year Alt mean</t>
+  </si>
+  <si>
+    <t>Ten Year Alt std</t>
   </si>
   <si>
     <t>LR</t>
@@ -43,16 +58,13 @@
     <t>KNN</t>
   </si>
   <si>
-    <t>CART</t>
+    <t>DTREE</t>
   </si>
   <si>
     <t>RTREE</t>
   </si>
   <si>
     <t>XTREE</t>
-  </si>
-  <si>
-    <t>NB</t>
   </si>
   <si>
     <t>SVM</t>
@@ -413,13 +425,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,189 +450,286 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>0.9025555328489057</v>
+        <v>0.9090633192976881</v>
       </c>
       <c r="D2">
-        <v>0.890372606161532</v>
+        <v>0.007655612320712047</v>
       </c>
       <c r="E2">
-        <v>0.8808988764044944</v>
+        <v>0.8944535291078293</v>
       </c>
       <c r="F2">
-        <v>0.8650730821923786</v>
+        <v>0.004195076109444465</v>
       </c>
       <c r="G2">
-        <v>0.8554356987735806</v>
+        <v>0.882236415073543</v>
+      </c>
+      <c r="H2">
+        <v>0.01079074962255617</v>
+      </c>
+      <c r="I2">
+        <v>0.8722299793778999</v>
+      </c>
+      <c r="J2">
+        <v>0.01990929111612589</v>
+      </c>
+      <c r="K2">
+        <v>0.8608850808732044</v>
+      </c>
+      <c r="L2">
+        <v>0.01811944010881063</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0.8962846603358227</v>
+        <v>0.9141068827626387</v>
       </c>
       <c r="D3">
-        <v>0.8863734388009992</v>
+        <v>0.008389764514451451</v>
       </c>
       <c r="E3">
-        <v>0.8791702679343129</v>
+        <v>0.9015338886333828</v>
       </c>
       <c r="F3">
-        <v>0.8676897300976465</v>
+        <v>0.008642836735566218</v>
       </c>
       <c r="G3">
-        <v>0.8566088553692573</v>
+        <v>0.8888877322327409</v>
+      </c>
+      <c r="H3">
+        <v>0.01071340011758976</v>
+      </c>
+      <c r="I3">
+        <v>0.8777206135074757</v>
+      </c>
+      <c r="J3">
+        <v>0.01816703426875145</v>
+      </c>
+      <c r="K3">
+        <v>0.8627898427779662</v>
+      </c>
+      <c r="L3">
+        <v>0.01175707424204308</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>0.886636805984898</v>
+        <v>0.8976756441831519</v>
       </c>
       <c r="D4">
-        <v>0.895703164029975</v>
+        <v>0.00860070140328904</v>
       </c>
       <c r="E4">
-        <v>0.8923076923076924</v>
+        <v>0.8959715195802886</v>
       </c>
       <c r="F4">
-        <v>0.891980941909474</v>
+        <v>0.0147702220321703</v>
       </c>
       <c r="G4">
-        <v>0.8877690257007229</v>
+        <v>0.8866104123547205</v>
+      </c>
+      <c r="H4">
+        <v>0.01274066556905293</v>
+      </c>
+      <c r="I4">
+        <v>0.8909710288136565</v>
+      </c>
+      <c r="J4">
+        <v>0.01402472819133107</v>
+      </c>
+      <c r="K4">
+        <v>0.8839503449835991</v>
+      </c>
+      <c r="L4">
+        <v>0.01400964459002119</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>0.8869584787349349</v>
+        <v>0.8874290935091762</v>
       </c>
       <c r="D5">
-        <v>0.8835406605606438</v>
+        <v>0.01234268693575006</v>
       </c>
       <c r="E5">
-        <v>0.8824546240276577</v>
+        <v>0.8850125765808734</v>
       </c>
       <c r="F5">
-        <v>0.8790870616159235</v>
+        <v>0.0095418996474835</v>
       </c>
       <c r="G5">
-        <v>0.8894111154734221</v>
+        <v>0.8850394351707835</v>
+      </c>
+      <c r="H5">
+        <v>0.01489291970865616</v>
+      </c>
+      <c r="I5">
+        <v>0.8775333677035</v>
+      </c>
+      <c r="J5">
+        <v>0.01458242444907673</v>
+      </c>
+      <c r="K5">
+        <v>0.8856187082909173</v>
+      </c>
+      <c r="L5">
+        <v>0.01298724687587197</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>0.8998211204610772</v>
+        <v>0.9093882577262253</v>
       </c>
       <c r="D6">
-        <v>0.8888730224812657</v>
+        <v>0.006807428383615113</v>
       </c>
       <c r="E6">
-        <v>0.8732929991356958</v>
+        <v>0.8976553051595211</v>
       </c>
       <c r="F6">
-        <v>0.8635770569910207</v>
+        <v>0.007481318467676062</v>
       </c>
       <c r="G6">
-        <v>0.8441936573218646</v>
+        <v>0.8857396543911431</v>
+      </c>
+      <c r="H6">
+        <v>0.008423643936893786</v>
+      </c>
+      <c r="I6">
+        <v>0.8739330927421664</v>
+      </c>
+      <c r="J6">
+        <v>0.01699277216502831</v>
+      </c>
+      <c r="K6">
+        <v>0.8635058251329035</v>
+      </c>
+      <c r="L6">
+        <v>0.01674456319474749</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>0.9167062883336395</v>
+        <v>0.9173618283414104</v>
       </c>
       <c r="D7">
-        <v>0.9061990008326395</v>
+        <v>0.009721805478364327</v>
       </c>
       <c r="E7">
-        <v>0.8834917891097668</v>
+        <v>0.9087843017016709</v>
       </c>
       <c r="F7">
-        <v>0.8704911995951028</v>
+        <v>0.009730136102976808</v>
       </c>
       <c r="G7">
-        <v>0.8769917991604229</v>
+        <v>0.8990358590621288</v>
+      </c>
+      <c r="H7">
+        <v>0.01108614190671006</v>
+      </c>
+      <c r="I7">
+        <v>0.8994919659735349</v>
+      </c>
+      <c r="J7">
+        <v>0.01578586165891406</v>
+      </c>
+      <c r="K7">
+        <v>0.8970320099536252</v>
+      </c>
+      <c r="L7">
+        <v>0.009927898663925837</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>0.8309976382209829</v>
+        <v>0.908899393554196</v>
       </c>
       <c r="D8">
-        <v>0.8155646683319455</v>
+        <v>0.005620607179130398</v>
       </c>
       <c r="E8">
-        <v>0.8057044079515989</v>
+        <v>0.9057511597140602</v>
       </c>
       <c r="F8">
-        <v>0.7983584212501199</v>
+        <v>0.00910680787134438</v>
       </c>
       <c r="G8">
-        <v>0.7563304606142806</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>0.9011081994862549</v>
-      </c>
-      <c r="D9">
-        <v>0.900868581737441</v>
-      </c>
-      <c r="E9">
-        <v>0.8961106309420916</v>
-      </c>
-      <c r="F9">
-        <v>0.8944115465500844</v>
-      </c>
-      <c r="G9">
-        <v>0.8915202165658606</v>
+        <v>0.9007874787209289</v>
+      </c>
+      <c r="H8">
+        <v>0.008782040317103978</v>
+      </c>
+      <c r="I8">
+        <v>0.8979775305035229</v>
+      </c>
+      <c r="J8">
+        <v>0.01592426866106061</v>
+      </c>
+      <c r="K8">
+        <v>0.8891884402216945</v>
+      </c>
+      <c r="L8">
+        <v>0.01338668063846961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>